<commit_message>
chore: add example xlsx files for repo
</commit_message>
<xml_diff>
--- a/xlsx_files_examples/Dienstplan_Template.xlsx
+++ b/xlsx_files_examples/Dienstplan_Template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ilianamarquez/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ilianamarquez/Documents/vscode-projects/schedule-maker-api/xlsx_files_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{D115D4B1-8501-B14F-903A-10E822E8D2A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED9D6412-1D06-D441-8502-99E7FCB52C2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="980" yWindow="1400" windowWidth="34920" windowHeight="19760" tabRatio="500" xr2:uid="{F0B8F572-F747-FE40-ABD3-2F8E2D1D428C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="40">
   <si>
     <t xml:space="preserve">Von </t>
   </si>
@@ -121,46 +121,7 @@
     <t>CG</t>
   </si>
   <si>
-    <t>Mo, 14.7.2025</t>
-  </si>
-  <si>
-    <t>Di, 15.7.2025</t>
-  </si>
-  <si>
-    <t>Mi, 16.7..2025</t>
-  </si>
-  <si>
-    <t>Do, 17.7.2025</t>
-  </si>
-  <si>
-    <t>Fr,18.7.2025</t>
-  </si>
-  <si>
-    <t>Mo, 21.7.2025</t>
-  </si>
-  <si>
-    <t>Di,22.7.2025</t>
-  </si>
-  <si>
-    <t>Mi, 23.7.2025</t>
-  </si>
-  <si>
-    <t>Do, 24.7.2025</t>
-  </si>
-  <si>
-    <t>Fr, 25.7.2025</t>
-  </si>
-  <si>
-    <t>Sa, 26.7.2025</t>
-  </si>
-  <si>
     <t>NG</t>
-  </si>
-  <si>
-    <t>Di, 29.7.2025</t>
-  </si>
-  <si>
-    <t>Do, 31.7.2025</t>
   </si>
   <si>
     <t>Arbeitstage</t>
@@ -218,12 +179,6 @@
   </si>
   <si>
     <t>-</t>
-  </si>
-  <si>
-    <t>Mi, 30.7.2025</t>
-  </si>
-  <si>
-    <t>Mo, 28.7.2025</t>
   </si>
 </sst>
 </file>
@@ -413,7 +368,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -421,22 +376,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="20" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="20" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
@@ -445,10 +391,19 @@
     <xf numFmtId="14" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -921,7 +876,7 @@
   <dimension ref="A1:AN1003"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="S44" sqref="S44:U44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1073,41 +1028,41 @@
       </c>
     </row>
     <row r="4" spans="1:40" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="37"/>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
+      <c r="A4" s="39"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="41"/>
       <c r="J4" s="8" t="s">
         <v>5</v>
       </c>
       <c r="K4" s="8"/>
       <c r="L4" s="8"/>
-      <c r="M4" s="37"/>
-      <c r="N4" s="37"/>
-      <c r="O4" s="37"/>
+      <c r="M4" s="39"/>
+      <c r="N4" s="39"/>
+      <c r="O4" s="39"/>
       <c r="P4" s="8"/>
       <c r="Q4" s="8"/>
       <c r="R4" s="8"/>
-      <c r="S4" s="38"/>
-      <c r="T4" s="38"/>
-      <c r="U4" s="38"/>
+      <c r="S4" s="41"/>
+      <c r="T4" s="41"/>
+      <c r="U4" s="41"/>
       <c r="V4" s="8"/>
       <c r="W4" s="8"/>
       <c r="X4" s="8"/>
-      <c r="Y4" s="39"/>
-      <c r="Z4" s="39"/>
-      <c r="AA4" s="39"/>
+      <c r="Y4" s="40"/>
+      <c r="Z4" s="40"/>
+      <c r="AA4" s="40"/>
       <c r="AB4" s="8"/>
       <c r="AC4" s="8"/>
       <c r="AD4" s="8"/>
-      <c r="AE4" s="37"/>
-      <c r="AF4" s="37"/>
-      <c r="AG4" s="37"/>
+      <c r="AE4" s="39"/>
+      <c r="AF4" s="39"/>
+      <c r="AG4" s="39"/>
       <c r="AH4" s="8"/>
       <c r="AI4" s="9"/>
       <c r="AJ4" s="9"/>
@@ -1781,10 +1736,10 @@
       </c>
     </row>
     <row r="11" spans="1:40" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="40" t="s">
+      <c r="A11" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="40"/>
+      <c r="B11" s="37"/>
       <c r="C11" s="12"/>
       <c r="D11" s="18">
         <f>SUM(D5:D10)</f>
@@ -1792,10 +1747,10 @@
       </c>
       <c r="E11" s="19"/>
       <c r="F11" s="19"/>
-      <c r="G11" s="40" t="s">
+      <c r="G11" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="H11" s="40"/>
+      <c r="H11" s="37"/>
       <c r="I11" s="12"/>
       <c r="J11" s="18">
         <f>SUM(J5:J10)</f>
@@ -1803,10 +1758,10 @@
       </c>
       <c r="K11" s="19"/>
       <c r="L11" s="19"/>
-      <c r="M11" s="40" t="s">
+      <c r="M11" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="N11" s="40"/>
+      <c r="N11" s="37"/>
       <c r="O11" s="12"/>
       <c r="P11" s="18">
         <f>SUM(P5:P10)</f>
@@ -1814,10 +1769,10 @@
       </c>
       <c r="Q11" s="19"/>
       <c r="R11" s="19"/>
-      <c r="S11" s="40" t="s">
+      <c r="S11" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="T11" s="40"/>
+      <c r="T11" s="37"/>
       <c r="U11" s="12"/>
       <c r="V11" s="18">
         <f>SUM(V5:V10)</f>
@@ -1825,10 +1780,10 @@
       </c>
       <c r="W11" s="19"/>
       <c r="X11" s="19"/>
-      <c r="Y11" s="40" t="s">
+      <c r="Y11" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="Z11" s="40"/>
+      <c r="Z11" s="37"/>
       <c r="AA11" s="12"/>
       <c r="AB11" s="18">
         <f>SUM(AB5:AB10)</f>
@@ -1836,10 +1791,10 @@
       </c>
       <c r="AC11" s="19"/>
       <c r="AD11" s="20"/>
-      <c r="AE11" s="40" t="s">
+      <c r="AE11" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="AF11" s="40"/>
+      <c r="AF11" s="37"/>
       <c r="AG11" s="12"/>
       <c r="AH11" s="18">
         <f>SUM(AH5:AH10)</f>
@@ -1853,39 +1808,39 @@
       <c r="AN11" s="10"/>
     </row>
     <row r="12" spans="1:40" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="39"/>
-      <c r="B12" s="39"/>
-      <c r="C12" s="39"/>
+      <c r="A12" s="40"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="40"/>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="41"/>
-      <c r="I12" s="41"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
       <c r="L12" s="8"/>
-      <c r="M12" s="42"/>
-      <c r="N12" s="42"/>
-      <c r="O12" s="42"/>
+      <c r="M12" s="43"/>
+      <c r="N12" s="43"/>
+      <c r="O12" s="43"/>
       <c r="P12" s="8"/>
       <c r="Q12" s="8"/>
       <c r="R12" s="8"/>
-      <c r="S12" s="39"/>
-      <c r="T12" s="39"/>
-      <c r="U12" s="39"/>
+      <c r="S12" s="40"/>
+      <c r="T12" s="40"/>
+      <c r="U12" s="40"/>
       <c r="V12" s="8"/>
       <c r="W12" s="8"/>
       <c r="X12" s="8"/>
-      <c r="Y12" s="43"/>
-      <c r="Z12" s="43"/>
-      <c r="AA12" s="43"/>
+      <c r="Y12" s="42"/>
+      <c r="Z12" s="42"/>
+      <c r="AA12" s="42"/>
       <c r="AB12" s="8"/>
       <c r="AC12" s="8"/>
       <c r="AD12" s="8"/>
-      <c r="AE12" s="37"/>
-      <c r="AF12" s="37"/>
-      <c r="AG12" s="37"/>
+      <c r="AE12" s="39"/>
+      <c r="AF12" s="39"/>
+      <c r="AG12" s="39"/>
       <c r="AH12" s="9"/>
       <c r="AI12" s="9"/>
       <c r="AJ12" s="9"/>
@@ -2611,10 +2566,10 @@
       </c>
     </row>
     <row r="19" spans="1:40" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="40" t="s">
+      <c r="A19" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="40"/>
+      <c r="B19" s="37"/>
       <c r="C19" s="12"/>
       <c r="D19" s="18">
         <f>SUM(D13:D18)</f>
@@ -2622,10 +2577,10 @@
       </c>
       <c r="E19" s="19"/>
       <c r="F19" s="19"/>
-      <c r="G19" s="40" t="s">
+      <c r="G19" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="H19" s="40"/>
+      <c r="H19" s="37"/>
       <c r="I19" s="12"/>
       <c r="J19" s="18">
         <f>SUM(J13:J18)</f>
@@ -2633,10 +2588,10 @@
       </c>
       <c r="K19" s="19"/>
       <c r="L19" s="19"/>
-      <c r="M19" s="40" t="s">
+      <c r="M19" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="N19" s="40"/>
+      <c r="N19" s="37"/>
       <c r="O19" s="12"/>
       <c r="P19" s="18">
         <f>SUM(P13:P18)</f>
@@ -2644,10 +2599,10 @@
       </c>
       <c r="Q19" s="19"/>
       <c r="R19" s="19"/>
-      <c r="S19" s="40" t="s">
+      <c r="S19" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="T19" s="40"/>
+      <c r="T19" s="37"/>
       <c r="U19" s="12"/>
       <c r="V19" s="18">
         <f>SUM(V13:V18)</f>
@@ -2655,10 +2610,10 @@
       </c>
       <c r="W19" s="19"/>
       <c r="X19" s="19"/>
-      <c r="Y19" s="40" t="s">
+      <c r="Y19" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="Z19" s="40"/>
+      <c r="Z19" s="37"/>
       <c r="AA19" s="12"/>
       <c r="AB19" s="18">
         <f>SUM(AB13:AB18)</f>
@@ -2666,10 +2621,10 @@
       </c>
       <c r="AC19" s="19"/>
       <c r="AD19" s="20"/>
-      <c r="AE19" s="40" t="s">
+      <c r="AE19" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="AF19" s="40"/>
+      <c r="AF19" s="37"/>
       <c r="AG19" s="12"/>
       <c r="AH19" s="18">
         <f>SUM(AH13:AH18)</f>
@@ -2683,39 +2638,39 @@
       <c r="AN19" s="10"/>
     </row>
     <row r="20" spans="1:40" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="37"/>
-      <c r="B20" s="37"/>
-      <c r="C20" s="37"/>
+      <c r="A20" s="39"/>
+      <c r="B20" s="39"/>
+      <c r="C20" s="39"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
-      <c r="G20" s="39"/>
-      <c r="H20" s="39"/>
-      <c r="I20" s="39"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="40"/>
+      <c r="I20" s="40"/>
       <c r="J20" s="8"/>
       <c r="K20" s="8"/>
       <c r="L20" s="8"/>
-      <c r="M20" s="37"/>
-      <c r="N20" s="37"/>
-      <c r="O20" s="37"/>
+      <c r="M20" s="39"/>
+      <c r="N20" s="39"/>
+      <c r="O20" s="39"/>
       <c r="P20" s="8"/>
       <c r="Q20" s="8"/>
       <c r="R20" s="8"/>
-      <c r="S20" s="41"/>
-      <c r="T20" s="41"/>
-      <c r="U20" s="41"/>
+      <c r="S20" s="38"/>
+      <c r="T20" s="38"/>
+      <c r="U20" s="38"/>
       <c r="V20" s="8"/>
       <c r="W20" s="8"/>
       <c r="X20" s="8"/>
-      <c r="Y20" s="43"/>
-      <c r="Z20" s="43"/>
-      <c r="AA20" s="43"/>
+      <c r="Y20" s="42"/>
+      <c r="Z20" s="42"/>
+      <c r="AA20" s="42"/>
       <c r="AB20" s="8"/>
       <c r="AC20" s="8"/>
       <c r="AD20" s="8"/>
-      <c r="AE20" s="37"/>
-      <c r="AF20" s="37"/>
-      <c r="AG20" s="37"/>
+      <c r="AE20" s="39"/>
+      <c r="AF20" s="39"/>
+      <c r="AG20" s="39"/>
       <c r="AH20" s="9"/>
       <c r="AI20" s="9"/>
       <c r="AJ20" s="9"/>
@@ -3441,10 +3396,10 @@
       </c>
     </row>
     <row r="27" spans="1:40" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="40" t="s">
+      <c r="A27" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="B27" s="40"/>
+      <c r="B27" s="37"/>
       <c r="C27" s="12"/>
       <c r="D27" s="18">
         <f>SUM(D21:D26)</f>
@@ -3452,10 +3407,10 @@
       </c>
       <c r="E27" s="19"/>
       <c r="F27" s="19"/>
-      <c r="G27" s="40" t="s">
+      <c r="G27" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="H27" s="40"/>
+      <c r="H27" s="37"/>
       <c r="I27" s="12"/>
       <c r="J27" s="18">
         <f>SUM(J21:J26)</f>
@@ -3463,10 +3418,10 @@
       </c>
       <c r="K27" s="19"/>
       <c r="L27" s="19"/>
-      <c r="M27" s="40" t="s">
+      <c r="M27" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="N27" s="40"/>
+      <c r="N27" s="37"/>
       <c r="O27" s="12"/>
       <c r="P27" s="18">
         <f>SUM(P21:P26)</f>
@@ -3474,10 +3429,10 @@
       </c>
       <c r="Q27" s="19"/>
       <c r="R27" s="19"/>
-      <c r="S27" s="40" t="s">
+      <c r="S27" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="T27" s="40"/>
+      <c r="T27" s="37"/>
       <c r="U27" s="12"/>
       <c r="V27" s="18">
         <f>SUM(V21:V26)</f>
@@ -3485,10 +3440,10 @@
       </c>
       <c r="W27" s="19"/>
       <c r="X27" s="19"/>
-      <c r="Y27" s="40" t="s">
+      <c r="Y27" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="Z27" s="40"/>
+      <c r="Z27" s="37"/>
       <c r="AA27" s="12"/>
       <c r="AB27" s="18">
         <f>SUM(AB21:AB26)</f>
@@ -3496,10 +3451,10 @@
       </c>
       <c r="AC27" s="19"/>
       <c r="AD27" s="20"/>
-      <c r="AE27" s="40" t="s">
+      <c r="AE27" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="AF27" s="40"/>
+      <c r="AF27" s="37"/>
       <c r="AG27" s="12"/>
       <c r="AH27" s="18">
         <f>SUM(AH21:AH26)</f>
@@ -3513,49 +3468,39 @@
       <c r="AN27" s="10"/>
     </row>
     <row r="28" spans="1:40" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="37" t="s">
-        <v>20</v>
-      </c>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
+      <c r="A28" s="39"/>
+      <c r="B28" s="39"/>
+      <c r="C28" s="39"/>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
       <c r="F28" s="8"/>
-      <c r="G28" s="39" t="s">
-        <v>21</v>
-      </c>
-      <c r="H28" s="39"/>
-      <c r="I28" s="39"/>
+      <c r="G28" s="40"/>
+      <c r="H28" s="40"/>
+      <c r="I28" s="40"/>
       <c r="J28" s="8"/>
       <c r="K28" s="8"/>
       <c r="L28" s="8"/>
-      <c r="M28" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="N28" s="37"/>
-      <c r="O28" s="37"/>
+      <c r="M28" s="39"/>
+      <c r="N28" s="39"/>
+      <c r="O28" s="39"/>
       <c r="P28" s="8"/>
       <c r="Q28" s="8"/>
       <c r="R28" s="8"/>
-      <c r="S28" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="T28" s="39"/>
-      <c r="U28" s="39"/>
+      <c r="S28" s="40"/>
+      <c r="T28" s="40"/>
+      <c r="U28" s="40"/>
       <c r="V28" s="8"/>
       <c r="W28" s="8"/>
       <c r="X28" s="8"/>
-      <c r="Y28" s="39" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z28" s="39"/>
-      <c r="AA28" s="39"/>
+      <c r="Y28" s="40"/>
+      <c r="Z28" s="40"/>
+      <c r="AA28" s="40"/>
       <c r="AB28" s="8"/>
       <c r="AC28" s="8"/>
       <c r="AD28" s="8"/>
-      <c r="AE28" s="37"/>
-      <c r="AF28" s="37"/>
-      <c r="AG28" s="37"/>
+      <c r="AE28" s="39"/>
+      <c r="AF28" s="39"/>
+      <c r="AG28" s="39"/>
       <c r="AH28" s="9"/>
       <c r="AI28" s="9"/>
       <c r="AJ28" s="9"/>
@@ -4281,10 +4226,10 @@
       </c>
     </row>
     <row r="35" spans="1:40" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="40" t="s">
+      <c r="A35" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="B35" s="40"/>
+      <c r="B35" s="37"/>
       <c r="C35" s="23"/>
       <c r="D35" s="18">
         <f>SUM(D29:D34)</f>
@@ -4292,10 +4237,10 @@
       </c>
       <c r="E35" s="19"/>
       <c r="F35" s="19"/>
-      <c r="G35" s="40" t="s">
+      <c r="G35" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="H35" s="40"/>
+      <c r="H35" s="37"/>
       <c r="I35" s="12"/>
       <c r="J35" s="18">
         <f>SUM(J29:J34)</f>
@@ -4303,10 +4248,10 @@
       </c>
       <c r="K35" s="19"/>
       <c r="L35" s="19"/>
-      <c r="M35" s="40" t="s">
+      <c r="M35" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="N35" s="40"/>
+      <c r="N35" s="37"/>
       <c r="O35" s="12"/>
       <c r="P35" s="18">
         <f>SUM(P29:P34)</f>
@@ -4325,10 +4270,10 @@
       </c>
       <c r="W35" s="19"/>
       <c r="X35" s="19"/>
-      <c r="Y35" s="40" t="s">
+      <c r="Y35" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="Z35" s="40"/>
+      <c r="Z35" s="37"/>
       <c r="AA35" s="12"/>
       <c r="AB35" s="18">
         <f>SUM(AB29:AB34)</f>
@@ -4336,10 +4281,10 @@
       </c>
       <c r="AC35" s="19"/>
       <c r="AD35" s="20"/>
-      <c r="AE35" s="40" t="s">
+      <c r="AE35" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="AF35" s="40"/>
+      <c r="AF35" s="37"/>
       <c r="AG35" s="12"/>
       <c r="AH35" s="18">
         <f>SUM(AH29:AH34)</f>
@@ -4353,51 +4298,39 @@
       <c r="AN35" s="10"/>
     </row>
     <row r="36" spans="1:40" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="37" t="s">
-        <v>25</v>
-      </c>
-      <c r="B36" s="37"/>
-      <c r="C36" s="37"/>
+      <c r="A36" s="39"/>
+      <c r="B36" s="39"/>
+      <c r="C36" s="39"/>
       <c r="D36" s="8"/>
       <c r="E36" s="8"/>
       <c r="F36" s="8"/>
-      <c r="G36" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="H36" s="39"/>
-      <c r="I36" s="39"/>
+      <c r="G36" s="40"/>
+      <c r="H36" s="40"/>
+      <c r="I36" s="40"/>
       <c r="J36" s="8"/>
       <c r="K36" s="8"/>
       <c r="L36" s="8"/>
-      <c r="M36" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="N36" s="37"/>
-      <c r="O36" s="37"/>
+      <c r="M36" s="39"/>
+      <c r="N36" s="39"/>
+      <c r="O36" s="39"/>
       <c r="P36" s="8"/>
       <c r="Q36" s="8"/>
       <c r="R36" s="8"/>
-      <c r="S36" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="T36" s="39"/>
-      <c r="U36" s="39"/>
+      <c r="S36" s="40"/>
+      <c r="T36" s="40"/>
+      <c r="U36" s="40"/>
       <c r="V36" s="8"/>
       <c r="W36" s="8"/>
       <c r="X36" s="8"/>
-      <c r="Y36" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z36" s="39"/>
-      <c r="AA36" s="39"/>
+      <c r="Y36" s="40"/>
+      <c r="Z36" s="40"/>
+      <c r="AA36" s="40"/>
       <c r="AB36" s="8"/>
       <c r="AC36" s="8"/>
       <c r="AD36" s="8"/>
-      <c r="AE36" s="41" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF36" s="41"/>
-      <c r="AG36" s="41"/>
+      <c r="AE36" s="38"/>
+      <c r="AF36" s="38"/>
+      <c r="AG36" s="38"/>
       <c r="AH36" s="9"/>
       <c r="AI36" s="9"/>
       <c r="AJ36" s="9"/>
@@ -5123,10 +5056,10 @@
       </c>
     </row>
     <row r="43" spans="1:40" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="40" t="s">
+      <c r="A43" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="B43" s="40"/>
+      <c r="B43" s="37"/>
       <c r="C43" s="12" t="s">
         <v>19</v>
       </c>
@@ -5136,10 +5069,10 @@
       </c>
       <c r="E43" s="19"/>
       <c r="F43" s="19"/>
-      <c r="G43" s="40" t="s">
+      <c r="G43" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="H43" s="40"/>
+      <c r="H43" s="37"/>
       <c r="I43" s="12"/>
       <c r="J43" s="18">
         <f>SUM(J37:J42)</f>
@@ -5147,10 +5080,10 @@
       </c>
       <c r="K43" s="19"/>
       <c r="L43" s="19"/>
-      <c r="M43" s="40" t="s">
+      <c r="M43" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="N43" s="40"/>
+      <c r="N43" s="37"/>
       <c r="O43" s="12"/>
       <c r="P43" s="18">
         <f>SUM(P37:P42)</f>
@@ -5158,10 +5091,10 @@
       </c>
       <c r="Q43" s="19"/>
       <c r="R43" s="19"/>
-      <c r="S43" s="40" t="s">
+      <c r="S43" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="T43" s="40"/>
+      <c r="T43" s="37"/>
       <c r="U43" s="12"/>
       <c r="V43" s="18">
         <f>SUM(V37:V42)</f>
@@ -5169,10 +5102,10 @@
       </c>
       <c r="W43" s="19"/>
       <c r="X43" s="19"/>
-      <c r="Y43" s="40" t="s">
+      <c r="Y43" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="Z43" s="40"/>
+      <c r="Z43" s="37"/>
       <c r="AA43" s="12"/>
       <c r="AB43" s="18">
         <f>SUM(AB37:AB42)</f>
@@ -5180,10 +5113,10 @@
       </c>
       <c r="AC43" s="19"/>
       <c r="AD43" s="20"/>
-      <c r="AE43" s="40" t="s">
+      <c r="AE43" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="AF43" s="40"/>
+      <c r="AF43" s="37"/>
       <c r="AG43" s="12"/>
       <c r="AH43" s="18">
         <f>SUM(AH37:AH42)</f>
@@ -5197,47 +5130,39 @@
       <c r="AN43" s="10"/>
     </row>
     <row r="44" spans="1:40" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="41" t="s">
-        <v>54</v>
-      </c>
-      <c r="B44" s="41"/>
-      <c r="C44" s="41"/>
+      <c r="A44" s="38"/>
+      <c r="B44" s="38"/>
+      <c r="C44" s="38"/>
       <c r="D44" s="8"/>
       <c r="E44" s="8"/>
       <c r="F44" s="8"/>
-      <c r="G44" s="37" t="s">
-        <v>32</v>
-      </c>
-      <c r="H44" s="37"/>
-      <c r="I44" s="37"/>
+      <c r="G44" s="39"/>
+      <c r="H44" s="39"/>
+      <c r="I44" s="39"/>
       <c r="J44" s="8"/>
       <c r="K44" s="8"/>
       <c r="L44" s="8"/>
-      <c r="M44" s="39" t="s">
-        <v>53</v>
-      </c>
-      <c r="N44" s="39"/>
-      <c r="O44" s="39"/>
+      <c r="M44" s="40"/>
+      <c r="N44" s="40"/>
+      <c r="O44" s="40"/>
       <c r="P44" s="8"/>
       <c r="Q44" s="8"/>
       <c r="R44" s="8"/>
-      <c r="S44" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="T44" s="39"/>
-      <c r="U44" s="39"/>
+      <c r="S44" s="40"/>
+      <c r="T44" s="40"/>
+      <c r="U44" s="40"/>
       <c r="V44" s="8"/>
       <c r="W44" s="8"/>
       <c r="X44" s="24"/>
-      <c r="Y44" s="38"/>
-      <c r="Z44" s="38"/>
-      <c r="AA44" s="38"/>
+      <c r="Y44" s="41"/>
+      <c r="Z44" s="41"/>
+      <c r="AA44" s="41"/>
       <c r="AB44" s="8"/>
       <c r="AC44" s="8"/>
       <c r="AD44" s="8"/>
-      <c r="AE44" s="38"/>
-      <c r="AF44" s="38"/>
-      <c r="AG44" s="38"/>
+      <c r="AE44" s="41"/>
+      <c r="AF44" s="41"/>
+      <c r="AG44" s="41"/>
       <c r="AH44" s="9"/>
       <c r="AI44" s="9"/>
       <c r="AJ44" s="9"/>
@@ -5963,12 +5888,12 @@
       </c>
     </row>
     <row r="51" spans="1:40" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="40" t="s">
+      <c r="A51" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="B51" s="40"/>
+      <c r="B51" s="37"/>
       <c r="C51" s="12" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="D51" s="18">
         <f>SUM(D45:D50)</f>
@@ -5976,10 +5901,10 @@
       </c>
       <c r="E51" s="19"/>
       <c r="F51" s="19"/>
-      <c r="G51" s="40" t="s">
+      <c r="G51" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="H51" s="40"/>
+      <c r="H51" s="37"/>
       <c r="I51" s="12"/>
       <c r="J51" s="18">
         <f>SUM(J45:J50)</f>
@@ -5987,10 +5912,10 @@
       </c>
       <c r="K51" s="19"/>
       <c r="L51" s="19"/>
-      <c r="M51" s="40" t="s">
+      <c r="M51" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="N51" s="40"/>
+      <c r="N51" s="37"/>
       <c r="O51" s="12"/>
       <c r="P51" s="18">
         <f>SUM(P45:P50)</f>
@@ -5998,10 +5923,10 @@
       </c>
       <c r="Q51" s="19"/>
       <c r="R51" s="19"/>
-      <c r="S51" s="40" t="s">
+      <c r="S51" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="T51" s="40"/>
+      <c r="T51" s="37"/>
       <c r="U51" s="12"/>
       <c r="V51" s="18">
         <f>SUM(V45:V50)</f>
@@ -6009,10 +5934,10 @@
       </c>
       <c r="W51" s="19"/>
       <c r="X51" s="19"/>
-      <c r="Y51" s="40" t="s">
+      <c r="Y51" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="Z51" s="40"/>
+      <c r="Z51" s="37"/>
       <c r="AA51" s="12"/>
       <c r="AB51" s="18">
         <f>SUM(AB45:AB50)</f>
@@ -6020,10 +5945,10 @@
       </c>
       <c r="AC51" s="19"/>
       <c r="AD51" s="19"/>
-      <c r="AE51" s="40" t="s">
+      <c r="AE51" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="AF51" s="40"/>
+      <c r="AF51" s="37"/>
       <c r="AG51" s="12"/>
       <c r="AH51" s="18">
         <f>SUM(AH45:AH50)</f>
@@ -6077,15 +6002,15 @@
     </row>
     <row r="53" spans="1:40" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="G53" s="25" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="H53" s="25"/>
       <c r="M53" s="25" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="N53" s="25"/>
       <c r="S53" s="25" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="T53" s="25"/>
       <c r="U53" s="3"/>
@@ -6093,7 +6018,7 @@
       <c r="W53" s="26"/>
       <c r="X53" s="26"/>
       <c r="Y53" s="25" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="Z53" s="25"/>
       <c r="AA53" s="3"/>
@@ -6101,7 +6026,7 @@
       <c r="AC53" s="3"/>
       <c r="AD53" s="3"/>
       <c r="AE53" s="25" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="AF53" s="25"/>
       <c r="AG53" s="3"/>
@@ -6109,13 +6034,13 @@
       <c r="AI53" s="3"/>
       <c r="AJ53" s="3"/>
       <c r="AK53" s="25" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="AM53" s="27" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="AN53" s="26" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
     </row>
     <row r="54" spans="1:40" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -6556,7 +6481,7 @@
     </row>
     <row r="62" spans="1:40" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="G62" s="25" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="H62" s="25"/>
       <c r="I62" s="31"/>
@@ -6564,7 +6489,7 @@
       <c r="K62" s="31"/>
       <c r="L62" s="31"/>
       <c r="M62" s="25" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="N62" s="25"/>
       <c r="O62" s="31"/>
@@ -6572,7 +6497,7 @@
       <c r="Q62" s="26"/>
       <c r="R62" s="26"/>
       <c r="S62" s="25" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="T62" s="25"/>
       <c r="V62" s="3"/>
@@ -6908,21 +6833,21 @@
     </row>
     <row r="73" spans="1:37" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="G73" s="34" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="H73" s="34"/>
       <c r="I73" s="34"/>
       <c r="M73" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="S73" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="Y73" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="AE73" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
     </row>
     <row r="74" spans="1:37" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7901,11 +7826,65 @@
   </sheetData>
   <sheetProtection password="C358" sheet="1"/>
   <mergeCells count="71">
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="G51:H51"/>
-    <mergeCell ref="M51:N51"/>
-    <mergeCell ref="S51:T51"/>
-    <mergeCell ref="Y51:Z51"/>
+    <mergeCell ref="AE4:AG4"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="S4:U4"/>
+    <mergeCell ref="Y4:AA4"/>
+    <mergeCell ref="AE12:AG12"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="S11:T11"/>
+    <mergeCell ref="Y11:Z11"/>
+    <mergeCell ref="AE11:AF11"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="S12:U12"/>
+    <mergeCell ref="Y12:AA12"/>
+    <mergeCell ref="AE20:AG20"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="S19:T19"/>
+    <mergeCell ref="Y19:Z19"/>
+    <mergeCell ref="AE19:AF19"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="M20:O20"/>
+    <mergeCell ref="S20:U20"/>
+    <mergeCell ref="Y20:AA20"/>
+    <mergeCell ref="AE28:AG28"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="S27:T27"/>
+    <mergeCell ref="Y27:Z27"/>
+    <mergeCell ref="AE27:AF27"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="M28:O28"/>
+    <mergeCell ref="S28:U28"/>
+    <mergeCell ref="Y28:AA28"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="M35:N35"/>
+    <mergeCell ref="Y35:Z35"/>
+    <mergeCell ref="AE35:AF35"/>
+    <mergeCell ref="AE36:AG36"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="M43:N43"/>
+    <mergeCell ref="S43:T43"/>
+    <mergeCell ref="Y43:Z43"/>
+    <mergeCell ref="AE43:AF43"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="G36:I36"/>
+    <mergeCell ref="M36:O36"/>
+    <mergeCell ref="S36:U36"/>
+    <mergeCell ref="Y36:AA36"/>
     <mergeCell ref="AE51:AF51"/>
     <mergeCell ref="A44:C44"/>
     <mergeCell ref="G44:I44"/>
@@ -7913,65 +7892,11 @@
     <mergeCell ref="S44:U44"/>
     <mergeCell ref="Y44:AA44"/>
     <mergeCell ref="AE44:AG44"/>
-    <mergeCell ref="AE36:AG36"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="M43:N43"/>
-    <mergeCell ref="S43:T43"/>
-    <mergeCell ref="Y43:Z43"/>
-    <mergeCell ref="AE43:AF43"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="M35:N35"/>
-    <mergeCell ref="Y35:Z35"/>
-    <mergeCell ref="AE35:AF35"/>
-    <mergeCell ref="A36:C36"/>
-    <mergeCell ref="G36:I36"/>
-    <mergeCell ref="M36:O36"/>
-    <mergeCell ref="S36:U36"/>
-    <mergeCell ref="Y36:AA36"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="G28:I28"/>
-    <mergeCell ref="M28:O28"/>
-    <mergeCell ref="S28:U28"/>
-    <mergeCell ref="Y28:AA28"/>
-    <mergeCell ref="AE28:AG28"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="S27:T27"/>
-    <mergeCell ref="Y27:Z27"/>
-    <mergeCell ref="AE27:AF27"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="M20:O20"/>
-    <mergeCell ref="S20:U20"/>
-    <mergeCell ref="Y20:AA20"/>
-    <mergeCell ref="AE20:AG20"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="S19:T19"/>
-    <mergeCell ref="Y19:Z19"/>
-    <mergeCell ref="AE19:AF19"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="M12:O12"/>
-    <mergeCell ref="S12:U12"/>
-    <mergeCell ref="Y12:AA12"/>
-    <mergeCell ref="AE12:AG12"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="S11:T11"/>
-    <mergeCell ref="Y11:Z11"/>
-    <mergeCell ref="AE11:AF11"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="M4:O4"/>
-    <mergeCell ref="S4:U4"/>
-    <mergeCell ref="Y4:AA4"/>
-    <mergeCell ref="AE4:AG4"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="G51:H51"/>
+    <mergeCell ref="M51:N51"/>
+    <mergeCell ref="S51:T51"/>
+    <mergeCell ref="Y51:Z51"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt=" - " sqref="C47:C50 I48:I50" xr:uid="{7E290947-9AA0-5B41-A2CC-7E08702C2EA7}">
@@ -8003,7 +7928,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="B1" s="35">
         <v>43796</v>
@@ -8012,7 +7937,7 @@
     <row r="2" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="3" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="B3" s="36">
         <v>0.77083333333333337</v>
@@ -8020,7 +7945,7 @@
     </row>
     <row r="4" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="B4" s="36">
         <v>0.54166666666666663</v>
@@ -8028,7 +7953,7 @@
     </row>
     <row r="6" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>16</v>
@@ -8041,12 +7966,12 @@
     </row>
     <row r="8" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="12" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="12" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>